<commit_message>
Fixed DOE-2.2 and 2.1e spreadsheets to fix Table B15.5.2.11b
</commit_message>
<xml_diff>
--- a/input/DOE21E/120/Std140_CE_b_Output.xlsx
+++ b/input/DOE21E/120/Std140_CE_b_Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\DOE21E\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A98DD3-253C-4C5F-A676-AEF6D2575CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F8CCD-00DD-4993-B54E-FC967977F796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="810" windowWidth="33600" windowHeight="20790" xr2:uid="{6C5182BB-48B8-4F6B-8426-D0FB240A2181}"/>
+    <workbookView xWindow="32655" yWindow="165" windowWidth="33600" windowHeight="20790" xr2:uid="{6C5182BB-48B8-4F6B-8426-D0FB240A2181}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -1618,7 +1618,7 @@
   <dimension ref="A1:AO214"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:A76"/>
+      <selection activeCell="X80" sqref="X80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4058,9 +4058,18 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="W79" s="23"/>
-      <c r="X79" s="30"/>
-      <c r="Y79" s="22"/>
+      <c r="W79" s="23">
+        <f t="shared" ref="W79:Y79" si="12">W163</f>
+        <v>0</v>
+      </c>
+      <c r="X79" s="30">
+        <f>U79</f>
+        <v>37370</v>
+      </c>
+      <c r="Y79" s="22">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
       <c r="Z79" s="23">
         <f t="shared" si="11"/>
         <v>19575</v>
@@ -4146,9 +4155,18 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="W80" s="23"/>
-      <c r="X80" s="30"/>
-      <c r="Y80" s="22"/>
+      <c r="W80" s="23">
+        <f t="shared" ref="W80:Y80" si="13">W164</f>
+        <v>0</v>
+      </c>
+      <c r="X80" s="30">
+        <f t="shared" ref="X80:X81" si="14">U80</f>
+        <v>37370</v>
+      </c>
+      <c r="Y80" s="22">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
       <c r="Z80" s="23">
         <f t="shared" si="11"/>
         <v>19766</v>
@@ -4234,9 +4252,18 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="W81" s="23"/>
-      <c r="X81" s="38"/>
-      <c r="Y81" s="39"/>
+      <c r="W81" s="23">
+        <f t="shared" ref="W81:Y81" si="15">W165</f>
+        <v>0</v>
+      </c>
+      <c r="X81" s="30">
+        <f t="shared" si="14"/>
+        <v>37370</v>
+      </c>
+      <c r="Y81" s="22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="Z81" s="23">
         <f t="shared" si="11"/>
         <v>19474</v>
@@ -4639,19 +4666,19 @@
         <v>1658.0667000000001</v>
       </c>
       <c r="G89" s="53">
-        <f t="shared" ref="G89:H104" si="12">G173</f>
+        <f t="shared" ref="G89:H104" si="16">G173</f>
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="H89" s="54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>3.5405819802909435</v>
       </c>
       <c r="I89" s="55">
-        <f t="shared" ref="I89:J104" si="13">(I173-32)/180*100</f>
+        <f t="shared" ref="I89:J104" si="17">(I173-32)/180*100</f>
         <v>17.777777777777779</v>
       </c>
       <c r="J89" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>23.833333333333336</v>
       </c>
       <c r="K89" s="55">
@@ -4673,99 +4700,99 @@
         <v>193</v>
       </c>
       <c r="Q89" s="25">
-        <f t="shared" ref="Q89:AN99" si="14">Q173</f>
+        <f t="shared" ref="Q89:AN99" si="18">Q173</f>
         <v>3.8570000000000002</v>
       </c>
       <c r="R89" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37376</v>
       </c>
       <c r="S89" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="T89" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.8010000000000002</v>
       </c>
       <c r="U89" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37956</v>
       </c>
       <c r="V89" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="W89" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>25.11</v>
       </c>
       <c r="X89" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37368</v>
       </c>
       <c r="Y89" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="Z89" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA89" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB89" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC89" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.37E-2</v>
       </c>
       <c r="AD89" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37941</v>
       </c>
       <c r="AE89" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="AF89" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG89" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH89" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI89" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>68.849999999999994</v>
       </c>
       <c r="AJ89" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37941</v>
       </c>
       <c r="AK89" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="AL89" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM89" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN89" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -4774,39 +4801,39 @@
         <v>149</v>
       </c>
       <c r="B90" s="21">
-        <f t="shared" ref="B90:B112" si="15">B174-C90</f>
+        <f t="shared" ref="B90:B112" si="19">B174-C90</f>
         <v>1941</v>
       </c>
       <c r="C90" s="22">
-        <f t="shared" ref="C90:C112" si="16">C174</f>
+        <f t="shared" ref="C90:C112" si="20">C174</f>
         <v>241</v>
       </c>
       <c r="D90" s="23">
-        <f t="shared" ref="D90:D112" si="17">D174*0.2931</f>
+        <f t="shared" ref="D90:D112" si="21">D174*0.2931</f>
         <v>7627.0482000000011</v>
       </c>
       <c r="E90" s="24">
-        <f t="shared" ref="E90:E112" si="18">D90-F90</f>
+        <f t="shared" ref="E90:E112" si="22">D90-F90</f>
         <v>6067.170000000001</v>
       </c>
       <c r="F90" s="24">
-        <f t="shared" ref="F90:F112" si="19">F174*0.2931</f>
+        <f t="shared" ref="F90:F112" si="23">F174*0.2931</f>
         <v>1559.8782000000001</v>
       </c>
       <c r="G90" s="53">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="H90" s="54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>3.4954391384051333</v>
       </c>
       <c r="I90" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>18.333333333333332</v>
       </c>
       <c r="J90" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>23.944444444444439</v>
       </c>
       <c r="K90" s="55">
@@ -4817,110 +4844,110 @@
         <v>1.12E-2</v>
       </c>
       <c r="M90" s="57">
-        <f t="shared" ref="M90:M112" si="20">M174</f>
+        <f t="shared" ref="M90:M112" si="24">M174</f>
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="N90" s="58">
-        <f t="shared" ref="N90:N112" si="21">N174*(14.696/29.921)*(6894.8/1)</f>
+        <f t="shared" ref="N90:N112" si="25">N174*(14.696/29.921)*(6894.8/1)</f>
         <v>101254.86534273588</v>
       </c>
       <c r="P90" s="10" t="s">
         <v>194</v>
       </c>
       <c r="Q90" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4.1280000000000001</v>
       </c>
       <c r="R90" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37376</v>
       </c>
       <c r="S90" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="T90" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.851</v>
       </c>
       <c r="U90" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37591</v>
       </c>
       <c r="V90" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="W90" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>26.72</v>
       </c>
       <c r="X90" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37457</v>
       </c>
       <c r="Y90" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Z90" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA90" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB90" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC90" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.89E-2</v>
       </c>
       <c r="AD90" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37544</v>
       </c>
       <c r="AE90" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="AF90" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG90" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH90" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI90" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>100.7</v>
       </c>
       <c r="AJ90" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37544</v>
       </c>
       <c r="AK90" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="AL90" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM90" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN90" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -4929,153 +4956,153 @@
         <v>150</v>
       </c>
       <c r="B91" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1894</v>
       </c>
       <c r="C91" s="22">
+        <f t="shared" si="20"/>
+        <v>237</v>
+      </c>
+      <c r="D91" s="23">
+        <f t="shared" si="21"/>
+        <v>7546.1526000000003</v>
+      </c>
+      <c r="E91" s="24">
+        <f t="shared" si="22"/>
+        <v>5878.1205</v>
+      </c>
+      <c r="F91" s="24">
+        <f t="shared" si="23"/>
+        <v>1668.0321000000001</v>
+      </c>
+      <c r="G91" s="53">
         <f t="shared" si="16"/>
-        <v>237</v>
-      </c>
-      <c r="D91" s="23">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="H91" s="54">
+        <f t="shared" si="16"/>
+        <v>3.541132144533083</v>
+      </c>
+      <c r="I91" s="55">
         <f t="shared" si="17"/>
-        <v>7546.1526000000003</v>
-      </c>
-      <c r="E91" s="24">
-        <f t="shared" si="18"/>
-        <v>5878.1205</v>
-      </c>
-      <c r="F91" s="24">
-        <f t="shared" si="19"/>
-        <v>1668.0321000000001</v>
-      </c>
-      <c r="G91" s="53">
-        <f t="shared" si="12"/>
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="H91" s="54">
-        <f t="shared" si="12"/>
-        <v>3.541132144533083</v>
-      </c>
-      <c r="I91" s="55">
-        <f t="shared" si="13"/>
         <v>17.777777777777779</v>
       </c>
       <c r="J91" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>23.833333333333336</v>
       </c>
       <c r="K91" s="55">
         <v>17.37</v>
       </c>
       <c r="L91" s="60">
-        <f t="shared" ref="L91:L112" si="22">L175</f>
+        <f t="shared" ref="L91:L112" si="26">L175</f>
         <v>1.14E-2</v>
       </c>
       <c r="M91" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="N91" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P91" s="10" t="s">
         <v>195</v>
       </c>
       <c r="Q91" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4.9669999999999996</v>
       </c>
       <c r="R91" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37531</v>
       </c>
       <c r="S91" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="T91" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.8050000000000002</v>
       </c>
       <c r="U91" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37956</v>
       </c>
       <c r="V91" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="W91" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>31.5</v>
       </c>
       <c r="X91" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37810</v>
       </c>
       <c r="Y91" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Z91" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>10.78</v>
       </c>
       <c r="AA91" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB91" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
       <c r="AC91" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="AD91" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37447</v>
       </c>
       <c r="AE91" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="AF91" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG91" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH91" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI91" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>83.67</v>
       </c>
       <c r="AJ91" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37733</v>
       </c>
       <c r="AK91" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>18</v>
       </c>
       <c r="AL91" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM91" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN91" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -5084,153 +5111,153 @@
         <v>151</v>
       </c>
       <c r="B92" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1890</v>
       </c>
       <c r="C92" s="22">
+        <f t="shared" si="20"/>
+        <v>236</v>
+      </c>
+      <c r="D92" s="23">
+        <f t="shared" si="21"/>
+        <v>7528.2735000000011</v>
+      </c>
+      <c r="E92" s="24">
+        <f t="shared" si="22"/>
+        <v>5873.4309000000012</v>
+      </c>
+      <c r="F92" s="24">
+        <f t="shared" si="23"/>
+        <v>1654.8426000000002</v>
+      </c>
+      <c r="G92" s="53">
         <f t="shared" si="16"/>
-        <v>236</v>
-      </c>
-      <c r="D92" s="23">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="H92" s="54">
+        <f t="shared" si="16"/>
+        <v>3.5410505644402641</v>
+      </c>
+      <c r="I92" s="55">
         <f t="shared" si="17"/>
-        <v>7528.2735000000011</v>
-      </c>
-      <c r="E92" s="24">
-        <f t="shared" si="18"/>
-        <v>5873.4309000000012</v>
-      </c>
-      <c r="F92" s="24">
-        <f t="shared" si="19"/>
-        <v>1654.8426000000002</v>
-      </c>
-      <c r="G92" s="53">
-        <f t="shared" si="12"/>
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="H92" s="54">
-        <f t="shared" si="12"/>
-        <v>3.5410505644402641</v>
-      </c>
-      <c r="I92" s="55">
-        <f t="shared" si="13"/>
         <v>17.777777777777779</v>
       </c>
       <c r="J92" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>23.833333333333336</v>
       </c>
       <c r="K92" s="55">
         <v>17.37</v>
       </c>
       <c r="L92" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.14E-2</v>
       </c>
       <c r="M92" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="N92" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P92" s="10" t="s">
         <v>196</v>
       </c>
       <c r="Q92" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>5.5949999999999998</v>
       </c>
       <c r="R92" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37531</v>
       </c>
       <c r="S92" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="T92" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.8010000000000002</v>
       </c>
       <c r="U92" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37956</v>
       </c>
       <c r="V92" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="W92" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>32</v>
       </c>
       <c r="X92" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37822</v>
       </c>
       <c r="Y92" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Z92" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA92" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB92" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC92" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.77E-2</v>
       </c>
       <c r="AD92" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37447</v>
       </c>
       <c r="AE92" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="AF92" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG92" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH92" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI92" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>77.94</v>
       </c>
       <c r="AJ92" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37882</v>
       </c>
       <c r="AK92" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="AL92" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM92" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN92" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -5239,153 +5266,153 @@
         <v>152</v>
       </c>
       <c r="B93" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1694</v>
       </c>
       <c r="C93" s="22">
+        <f t="shared" si="20"/>
+        <v>215</v>
+      </c>
+      <c r="D93" s="23">
+        <f t="shared" si="21"/>
+        <v>6753.0240000000003</v>
+      </c>
+      <c r="E93" s="24">
+        <f t="shared" si="22"/>
+        <v>5671.7781000000004</v>
+      </c>
+      <c r="F93" s="24">
+        <f t="shared" si="23"/>
+        <v>1081.2459000000001</v>
+      </c>
+      <c r="G93" s="53">
         <f t="shared" si="16"/>
-        <v>215</v>
-      </c>
-      <c r="D93" s="23">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H93" s="54">
+        <f t="shared" si="16"/>
+        <v>3.5374667365112624</v>
+      </c>
+      <c r="I93" s="55">
         <f t="shared" si="17"/>
-        <v>6753.0240000000003</v>
-      </c>
-      <c r="E93" s="24">
-        <f t="shared" si="18"/>
-        <v>5671.7781000000004</v>
-      </c>
-      <c r="F93" s="24">
-        <f t="shared" si="19"/>
-        <v>1081.2459000000001</v>
-      </c>
-      <c r="G93" s="53">
-        <f t="shared" si="12"/>
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H93" s="54">
-        <f t="shared" si="12"/>
-        <v>3.5374667365112624</v>
-      </c>
-      <c r="I93" s="55">
-        <f t="shared" si="13"/>
         <v>17.222222222222221</v>
       </c>
       <c r="J93" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>23.777777777777775</v>
       </c>
       <c r="K93" s="55">
         <v>16.940000000000001</v>
       </c>
       <c r="L93" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.03E-2</v>
       </c>
       <c r="M93" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>9.1999999999999998E-3</v>
       </c>
       <c r="N93" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P93" s="10" t="s">
         <v>197</v>
       </c>
       <c r="Q93" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>5.3390000000000004</v>
       </c>
       <c r="R93" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37531</v>
       </c>
       <c r="S93" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="T93" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.8010000000000002</v>
       </c>
       <c r="U93" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37956</v>
       </c>
       <c r="V93" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="W93" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>31.56</v>
       </c>
       <c r="X93" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37810</v>
       </c>
       <c r="Y93" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Z93" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA93" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB93" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC93" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.7399999999999999E-2</v>
       </c>
       <c r="AD93" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37447</v>
       </c>
       <c r="AE93" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="AF93" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG93" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH93" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI93" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>81.260000000000005</v>
       </c>
       <c r="AJ93" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37733</v>
       </c>
       <c r="AK93" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>18</v>
       </c>
       <c r="AL93" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM93" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN93" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -5394,153 +5421,153 @@
         <v>153</v>
       </c>
       <c r="B94" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>2133</v>
       </c>
       <c r="C94" s="22">
+        <f t="shared" si="20"/>
+        <v>259</v>
+      </c>
+      <c r="D94" s="23">
+        <f t="shared" si="21"/>
+        <v>8185.1106000000009</v>
+      </c>
+      <c r="E94" s="24">
+        <f t="shared" si="22"/>
+        <v>6438.5277000000006</v>
+      </c>
+      <c r="F94" s="24">
+        <f t="shared" si="23"/>
+        <v>1746.5829000000001</v>
+      </c>
+      <c r="G94" s="53">
         <f t="shared" si="16"/>
-        <v>259</v>
-      </c>
-      <c r="D94" s="23">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="H94" s="54">
+        <f t="shared" si="16"/>
+        <v>3.4218689799331106</v>
+      </c>
+      <c r="I94" s="55">
         <f t="shared" si="17"/>
-        <v>8185.1106000000009</v>
-      </c>
-      <c r="E94" s="24">
-        <f t="shared" si="18"/>
-        <v>6438.5277000000006</v>
-      </c>
-      <c r="F94" s="24">
-        <f t="shared" si="19"/>
-        <v>1746.5829000000001</v>
-      </c>
-      <c r="G94" s="53">
-        <f t="shared" si="12"/>
-        <v>9.1999999999999998E-3</v>
-      </c>
-      <c r="H94" s="54">
-        <f t="shared" si="12"/>
-        <v>3.4218689799331106</v>
-      </c>
-      <c r="I94" s="55">
-        <f t="shared" si="13"/>
         <v>19.444444444444446</v>
       </c>
       <c r="J94" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>24.111111111111114</v>
       </c>
       <c r="K94" s="55">
         <v>17.3</v>
       </c>
       <c r="L94" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="M94" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="N94" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P94" s="10" t="s">
         <v>198</v>
       </c>
       <c r="Q94" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3.863</v>
       </c>
       <c r="R94" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>38265</v>
       </c>
       <c r="S94" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="T94" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.8010000000000002</v>
       </c>
       <c r="U94" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37956</v>
       </c>
       <c r="V94" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="W94" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>34.94</v>
       </c>
       <c r="X94" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>38162</v>
       </c>
       <c r="Y94" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="Z94" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA94" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB94" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC94" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.9900000000000001E-2</v>
       </c>
       <c r="AD94" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37470</v>
       </c>
       <c r="AE94" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>22</v>
       </c>
       <c r="AF94" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG94" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH94" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI94" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>81.12</v>
       </c>
       <c r="AJ94" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37840</v>
       </c>
       <c r="AK94" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
       <c r="AL94" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM94" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN94" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -5549,153 +5576,153 @@
         <v>154</v>
       </c>
       <c r="B95" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3223</v>
       </c>
       <c r="C95" s="22">
+        <f t="shared" si="20"/>
+        <v>353</v>
+      </c>
+      <c r="D95" s="23">
+        <f t="shared" si="21"/>
+        <v>11232.764400000002</v>
+      </c>
+      <c r="E95" s="24">
+        <f t="shared" si="22"/>
+        <v>8347.781100000002</v>
+      </c>
+      <c r="F95" s="24">
+        <f t="shared" si="23"/>
+        <v>2884.9833000000003</v>
+      </c>
+      <c r="G95" s="53">
         <f t="shared" si="16"/>
-        <v>353</v>
-      </c>
-      <c r="D95" s="23">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="H95" s="54">
+        <f t="shared" si="16"/>
+        <v>3.1411533557046987</v>
+      </c>
+      <c r="I95" s="55">
         <f t="shared" si="17"/>
-        <v>11232.764400000002</v>
-      </c>
-      <c r="E95" s="24">
-        <f t="shared" si="18"/>
-        <v>8347.781100000002</v>
-      </c>
-      <c r="F95" s="24">
-        <f t="shared" si="19"/>
-        <v>2884.9833000000003</v>
-      </c>
-      <c r="G95" s="53">
-        <f t="shared" si="12"/>
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="H95" s="54">
-        <f t="shared" si="12"/>
-        <v>3.1411533557046987</v>
-      </c>
-      <c r="I95" s="55">
-        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="J95" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>24.944444444444446</v>
       </c>
       <c r="K95" s="55">
         <v>18.23</v>
       </c>
       <c r="L95" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.3299999999999999E-2</v>
       </c>
       <c r="M95" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.03E-2</v>
       </c>
       <c r="N95" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P95" s="10" t="s">
         <v>199</v>
       </c>
       <c r="Q95" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4.4269999999999996</v>
       </c>
       <c r="R95" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37533</v>
       </c>
       <c r="S95" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="T95" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.8010000000000002</v>
       </c>
       <c r="U95" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37956</v>
       </c>
       <c r="V95" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="W95" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>32.56</v>
       </c>
       <c r="X95" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>38188</v>
       </c>
       <c r="Y95" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Z95" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA95" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB95" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC95" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.37E-2</v>
       </c>
       <c r="AD95" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37941</v>
       </c>
       <c r="AE95" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="AF95" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG95" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH95" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI95" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>68.849999999999994</v>
       </c>
       <c r="AJ95" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37941</v>
       </c>
       <c r="AK95" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="AL95" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM95" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN95" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -5704,153 +5731,153 @@
         <v>155</v>
       </c>
       <c r="B96" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3145</v>
       </c>
       <c r="C96" s="22">
+        <f t="shared" si="20"/>
+        <v>335</v>
+      </c>
+      <c r="D96" s="23">
+        <f t="shared" si="21"/>
+        <v>10271.6895</v>
+      </c>
+      <c r="E96" s="24">
+        <f t="shared" si="22"/>
+        <v>9069.1002000000008</v>
+      </c>
+      <c r="F96" s="24">
+        <f t="shared" si="23"/>
+        <v>1202.5893000000001</v>
+      </c>
+      <c r="G96" s="53">
         <f t="shared" si="16"/>
-        <v>335</v>
-      </c>
-      <c r="D96" s="23">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="H96" s="54">
+        <f t="shared" si="16"/>
+        <v>2.9516349137931037</v>
+      </c>
+      <c r="I96" s="55">
         <f t="shared" si="17"/>
-        <v>10271.6895</v>
-      </c>
-      <c r="E96" s="24">
-        <f t="shared" si="18"/>
-        <v>9069.1002000000008</v>
-      </c>
-      <c r="F96" s="24">
-        <f t="shared" si="19"/>
-        <v>1202.5893000000001</v>
-      </c>
-      <c r="G96" s="53">
-        <f t="shared" si="12"/>
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="H96" s="54">
-        <f t="shared" si="12"/>
-        <v>2.9516349137931037</v>
-      </c>
-      <c r="I96" s="55">
-        <f t="shared" si="13"/>
         <v>27.222222222222221</v>
       </c>
       <c r="J96" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>25.277777777777779</v>
       </c>
       <c r="K96" s="55">
         <v>17.78</v>
       </c>
       <c r="L96" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.09E-2</v>
       </c>
       <c r="M96" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="N96" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P96" s="10" t="s">
         <v>200</v>
       </c>
       <c r="Q96" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4.7759999999999998</v>
       </c>
       <c r="R96" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37882</v>
       </c>
       <c r="S96" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="T96" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.7349999999999999</v>
       </c>
       <c r="U96" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37958</v>
       </c>
       <c r="V96" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="W96" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>28.83</v>
       </c>
       <c r="X96" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37517</v>
       </c>
       <c r="Y96" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="Z96" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA96" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB96" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC96" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="AD96" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37716</v>
       </c>
       <c r="AE96" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
       <c r="AF96" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG96" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH96" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI96" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>85.57</v>
       </c>
       <c r="AJ96" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37716</v>
       </c>
       <c r="AK96" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
       <c r="AL96" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM96" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN96" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -5859,153 +5886,153 @@
         <v>156</v>
       </c>
       <c r="B97" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4526</v>
       </c>
       <c r="C97" s="22">
+        <f t="shared" si="20"/>
+        <v>467</v>
+      </c>
+      <c r="D97" s="23">
+        <f t="shared" si="21"/>
+        <v>14844.049500000001</v>
+      </c>
+      <c r="E97" s="24">
+        <f t="shared" si="22"/>
+        <v>11875.239600000001</v>
+      </c>
+      <c r="F97" s="24">
+        <f t="shared" si="23"/>
+        <v>2968.8099000000002</v>
+      </c>
+      <c r="G97" s="53">
         <f t="shared" si="16"/>
-        <v>467</v>
-      </c>
-      <c r="D97" s="23">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="H97" s="54">
+        <f t="shared" si="16"/>
+        <v>2.9729720608852395</v>
+      </c>
+      <c r="I97" s="55">
         <f t="shared" si="17"/>
-        <v>14844.049500000001</v>
-      </c>
-      <c r="E97" s="24">
-        <f t="shared" si="18"/>
-        <v>11875.239600000001</v>
-      </c>
-      <c r="F97" s="24">
-        <f t="shared" si="19"/>
-        <v>2968.8099000000002</v>
-      </c>
-      <c r="G97" s="53">
-        <f t="shared" si="12"/>
-        <v>9.9000000000000008E-3</v>
-      </c>
-      <c r="H97" s="54">
-        <f t="shared" si="12"/>
-        <v>2.9729720608852395</v>
-      </c>
-      <c r="I97" s="55">
-        <f t="shared" si="13"/>
         <v>28.888888888888886</v>
       </c>
       <c r="J97" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>25.555555555555554</v>
       </c>
       <c r="K97" s="55">
         <v>18.28</v>
       </c>
       <c r="L97" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.17E-2</v>
       </c>
       <c r="M97" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.01E-2</v>
       </c>
       <c r="N97" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P97" s="10" t="s">
         <v>201</v>
       </c>
       <c r="Q97" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3.855</v>
       </c>
       <c r="R97" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37376</v>
       </c>
       <c r="S97" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="T97" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.8010000000000002</v>
       </c>
       <c r="U97" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37956</v>
       </c>
       <c r="V97" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="W97" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>25.11</v>
       </c>
       <c r="X97" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37368</v>
       </c>
       <c r="Y97" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="Z97" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA97" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB97" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC97" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6899999999999998E-2</v>
       </c>
       <c r="AD97" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37348</v>
       </c>
       <c r="AE97" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="AF97" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG97" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH97" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI97" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>84.79</v>
       </c>
       <c r="AJ97" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37348</v>
       </c>
       <c r="AK97" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="AL97" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM97" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN97" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -6014,153 +6041,153 @@
         <v>157</v>
       </c>
       <c r="B98" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4655</v>
       </c>
       <c r="C98" s="22">
+        <f t="shared" si="20"/>
+        <v>478</v>
+      </c>
+      <c r="D98" s="23">
+        <f t="shared" si="21"/>
+        <v>15392.732700000002</v>
+      </c>
+      <c r="E98" s="24">
+        <f t="shared" si="22"/>
+        <v>12041.134200000002</v>
+      </c>
+      <c r="F98" s="24">
+        <f t="shared" si="23"/>
+        <v>3351.5985000000005</v>
+      </c>
+      <c r="G98" s="53">
         <f t="shared" si="16"/>
-        <v>478</v>
-      </c>
-      <c r="D98" s="23">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="H98" s="54">
+        <f t="shared" si="16"/>
+        <v>2.9987790181180602</v>
+      </c>
+      <c r="I98" s="55">
         <f t="shared" si="17"/>
-        <v>15392.732700000002</v>
-      </c>
-      <c r="E98" s="24">
-        <f t="shared" si="18"/>
-        <v>12041.134200000002</v>
-      </c>
-      <c r="F98" s="24">
-        <f t="shared" si="19"/>
-        <v>3351.5985000000005</v>
-      </c>
-      <c r="G98" s="53">
-        <f t="shared" si="12"/>
-        <v>1.0200000000000001E-2</v>
-      </c>
-      <c r="H98" s="54">
-        <f t="shared" si="12"/>
-        <v>2.9987790181180602</v>
-      </c>
-      <c r="I98" s="55">
-        <f t="shared" si="13"/>
         <v>28.888888888888886</v>
       </c>
       <c r="J98" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>25.555555555555554</v>
       </c>
       <c r="K98" s="55">
         <v>18.600000000000001</v>
       </c>
       <c r="L98" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="M98" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="N98" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P98" s="10" t="s">
         <v>202</v>
       </c>
       <c r="Q98" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3.7589999999999999</v>
       </c>
       <c r="R98" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37891</v>
       </c>
       <c r="S98" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="T98" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.8010000000000002</v>
       </c>
       <c r="U98" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37956</v>
       </c>
       <c r="V98" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="W98" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>25.11</v>
       </c>
       <c r="X98" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37368</v>
       </c>
       <c r="Y98" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="Z98" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA98" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB98" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC98" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.41E-2</v>
       </c>
       <c r="AD98" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37363</v>
       </c>
       <c r="AE98" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="AF98" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG98" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36895</v>
       </c>
       <c r="AH98" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="AI98" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>71.53</v>
       </c>
       <c r="AJ98" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37363</v>
       </c>
       <c r="AK98" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="AL98" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11.97</v>
       </c>
       <c r="AM98" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37566</v>
       </c>
       <c r="AN98" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
     </row>
@@ -6169,153 +6196,153 @@
         <v>158</v>
       </c>
       <c r="B99" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>5456</v>
       </c>
       <c r="C99" s="22">
+        <f t="shared" si="20"/>
+        <v>536</v>
+      </c>
+      <c r="D99" s="23">
+        <f t="shared" si="21"/>
+        <v>17605.051500000001</v>
+      </c>
+      <c r="E99" s="24">
+        <f t="shared" si="22"/>
+        <v>12817.556100000002</v>
+      </c>
+      <c r="F99" s="24">
+        <f t="shared" si="23"/>
+        <v>4787.4954000000007</v>
+      </c>
+      <c r="G99" s="53">
         <f t="shared" si="16"/>
-        <v>536</v>
-      </c>
-      <c r="D99" s="23">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="H99" s="54">
+        <f t="shared" si="16"/>
+        <v>2.9380927069425904</v>
+      </c>
+      <c r="I99" s="55">
         <f t="shared" si="17"/>
-        <v>17605.051500000001</v>
-      </c>
-      <c r="E99" s="24">
-        <f t="shared" si="18"/>
-        <v>12817.556100000002</v>
-      </c>
-      <c r="F99" s="24">
-        <f t="shared" si="19"/>
-        <v>4787.4954000000007</v>
-      </c>
-      <c r="G99" s="53">
-        <f t="shared" si="12"/>
-        <v>1.0699999999999999E-2</v>
-      </c>
-      <c r="H99" s="54">
-        <f t="shared" si="12"/>
-        <v>2.9380927069425904</v>
-      </c>
-      <c r="I99" s="55">
-        <f t="shared" si="13"/>
         <v>31.111111111111111</v>
       </c>
       <c r="J99" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>25.888888888888882</v>
       </c>
       <c r="K99" s="55">
         <v>19.329999999999998</v>
       </c>
       <c r="L99" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.4800000000000001E-2</v>
       </c>
       <c r="M99" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="N99" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P99" s="10" t="s">
         <v>203</v>
       </c>
       <c r="Q99" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3.7589999999999999</v>
       </c>
       <c r="R99" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37891</v>
       </c>
       <c r="S99" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="T99" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.7349999999999999</v>
       </c>
       <c r="U99" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37958</v>
       </c>
       <c r="V99" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="W99" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>25.11</v>
       </c>
       <c r="X99" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37368</v>
       </c>
       <c r="Y99" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="Z99" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>8.83</v>
       </c>
       <c r="AA99" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>36897</v>
       </c>
       <c r="AB99" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AC99" s="53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="AD99" s="30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37713</v>
       </c>
       <c r="AE99" s="24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="AF99" s="53">
-        <f t="shared" ref="AF99:AN99" si="23">AF183</f>
+        <f t="shared" ref="AF99:AN99" si="27">AF183</f>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG99" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>36895</v>
       </c>
       <c r="AH99" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>24</v>
       </c>
       <c r="AI99" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>78.430000000000007</v>
       </c>
       <c r="AJ99" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>37713</v>
       </c>
       <c r="AK99" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
       <c r="AL99" s="59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>11.97</v>
       </c>
       <c r="AM99" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>37566</v>
       </c>
       <c r="AN99" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
     </row>
@@ -6324,153 +6351,153 @@
         <v>159</v>
       </c>
       <c r="B100" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>5015</v>
       </c>
       <c r="C100" s="22">
+        <f t="shared" si="20"/>
+        <v>498</v>
+      </c>
+      <c r="D100" s="23">
+        <f t="shared" si="21"/>
+        <v>16187.619900000002</v>
+      </c>
+      <c r="E100" s="24">
+        <f t="shared" si="22"/>
+        <v>12610.920600000001</v>
+      </c>
+      <c r="F100" s="24">
+        <f t="shared" si="23"/>
+        <v>3576.6993000000002</v>
+      </c>
+      <c r="G100" s="53">
         <f t="shared" si="16"/>
-        <v>498</v>
-      </c>
-      <c r="D100" s="23">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="H100" s="54">
+        <f t="shared" si="16"/>
+        <v>2.9362633593324872</v>
+      </c>
+      <c r="I100" s="55">
         <f t="shared" si="17"/>
-        <v>16187.619900000002</v>
-      </c>
-      <c r="E100" s="24">
-        <f t="shared" si="18"/>
-        <v>12610.920600000001</v>
-      </c>
-      <c r="F100" s="24">
-        <f t="shared" si="19"/>
-        <v>3576.6993000000002</v>
-      </c>
-      <c r="G100" s="53">
-        <f t="shared" si="12"/>
-        <v>1.0800000000000001E-2</v>
-      </c>
-      <c r="H100" s="54">
-        <f t="shared" si="12"/>
-        <v>2.9362633593324872</v>
-      </c>
-      <c r="I100" s="55">
-        <f t="shared" si="13"/>
         <v>30.555555555555557</v>
       </c>
       <c r="J100" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>25.833333333333336</v>
       </c>
       <c r="K100" s="55">
         <v>19.23</v>
       </c>
       <c r="L100" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.34E-2</v>
       </c>
       <c r="M100" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.12E-2</v>
       </c>
       <c r="N100" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P100" s="11" t="s">
         <v>204</v>
       </c>
       <c r="Q100" s="25">
-        <f t="shared" ref="Q100:AN108" si="24">Q184</f>
+        <f t="shared" ref="Q100:AN108" si="28">Q184</f>
         <v>3.7589999999999999</v>
       </c>
       <c r="R100" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37526</v>
       </c>
       <c r="S100" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="T100" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.7349999999999999</v>
       </c>
       <c r="U100" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37958</v>
       </c>
       <c r="V100" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>13</v>
       </c>
       <c r="W100" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>25.11</v>
       </c>
       <c r="X100" s="38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37368</v>
       </c>
       <c r="Y100" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="Z100" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>8.83</v>
       </c>
       <c r="AA100" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>36897</v>
       </c>
       <c r="AB100" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>6</v>
       </c>
       <c r="AC100" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.37E-2</v>
       </c>
       <c r="AD100" s="38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37941</v>
       </c>
       <c r="AE100" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="AF100" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="AG100" s="38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>36895</v>
       </c>
       <c r="AH100" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>24</v>
       </c>
       <c r="AI100" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>68.849999999999994</v>
       </c>
       <c r="AJ100" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37941</v>
       </c>
       <c r="AK100" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="AL100" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>11.97</v>
       </c>
       <c r="AM100" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37566</v>
       </c>
       <c r="AN100" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
     </row>
@@ -6479,117 +6506,117 @@
         <v>160</v>
       </c>
       <c r="B101" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>6036</v>
       </c>
       <c r="C101" s="22">
+        <f t="shared" si="20"/>
+        <v>600</v>
+      </c>
+      <c r="D101" s="23">
+        <f t="shared" si="21"/>
+        <v>19620.993300000002</v>
+      </c>
+      <c r="E101" s="24">
+        <f t="shared" si="22"/>
+        <v>17135.212200000002</v>
+      </c>
+      <c r="F101" s="24">
+        <f t="shared" si="23"/>
+        <v>2485.7811000000002</v>
+      </c>
+      <c r="G101" s="53">
         <f t="shared" si="16"/>
-        <v>600</v>
-      </c>
-      <c r="D101" s="23">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="H101" s="54">
+        <f t="shared" si="16"/>
+        <v>2.9567500452079569</v>
+      </c>
+      <c r="I101" s="55">
         <f t="shared" si="17"/>
-        <v>19620.993300000002</v>
-      </c>
-      <c r="E101" s="24">
-        <f t="shared" si="18"/>
-        <v>17135.212200000002</v>
-      </c>
-      <c r="F101" s="24">
-        <f t="shared" si="19"/>
-        <v>2485.7811000000002</v>
-      </c>
-      <c r="G101" s="53">
-        <f t="shared" si="12"/>
-        <v>1.0200000000000001E-2</v>
-      </c>
-      <c r="H101" s="54">
-        <f t="shared" si="12"/>
-        <v>2.9567500452079569</v>
-      </c>
-      <c r="I101" s="55">
-        <f t="shared" si="13"/>
         <v>31.111111111111111</v>
       </c>
       <c r="J101" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>25.944444444444446</v>
       </c>
       <c r="K101" s="55">
         <v>18.64</v>
       </c>
       <c r="L101" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.15E-2</v>
       </c>
       <c r="M101" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.04E-2</v>
       </c>
       <c r="N101" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P101" s="10" t="s">
         <v>213</v>
       </c>
       <c r="Q101" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>5.3010000000000002</v>
       </c>
       <c r="R101" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38273</v>
       </c>
       <c r="S101" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>9</v>
       </c>
       <c r="T101" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.6520000000000001</v>
       </c>
       <c r="U101" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38076</v>
       </c>
       <c r="V101" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="W101" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>25.11</v>
       </c>
       <c r="X101" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37002</v>
       </c>
       <c r="Y101" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="Z101" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.94</v>
       </c>
       <c r="AA101" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37975</v>
       </c>
       <c r="AB101" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>11</v>
       </c>
       <c r="AC101" s="53">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.18E-2</v>
       </c>
       <c r="AD101" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38083</v>
       </c>
       <c r="AE101" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="AF101" s="53"/>
@@ -6607,117 +6634,117 @@
         <v>161</v>
       </c>
       <c r="B102" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>6429</v>
       </c>
       <c r="C102" s="22">
+        <f t="shared" si="20"/>
+        <v>635</v>
+      </c>
+      <c r="D102" s="23">
+        <f t="shared" si="21"/>
+        <v>20819.186100000003</v>
+      </c>
+      <c r="E102" s="24">
+        <f t="shared" si="22"/>
+        <v>17639.051100000004</v>
+      </c>
+      <c r="F102" s="24">
+        <f t="shared" si="23"/>
+        <v>3180.1350000000002</v>
+      </c>
+      <c r="G102" s="53">
         <f t="shared" si="16"/>
-        <v>635</v>
-      </c>
-      <c r="D102" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="H102" s="54">
+        <f t="shared" si="16"/>
+        <v>2.9472234003397513</v>
+      </c>
+      <c r="I102" s="55">
         <f t="shared" si="17"/>
-        <v>20819.186100000003</v>
-      </c>
-      <c r="E102" s="24">
-        <f t="shared" si="18"/>
-        <v>17639.051100000004</v>
-      </c>
-      <c r="F102" s="24">
-        <f t="shared" si="19"/>
-        <v>3180.1350000000002</v>
-      </c>
-      <c r="G102" s="53">
-        <f t="shared" si="12"/>
-        <v>0.01</v>
-      </c>
-      <c r="H102" s="54">
-        <f t="shared" si="12"/>
-        <v>2.9472234003397513</v>
-      </c>
-      <c r="I102" s="55">
-        <f t="shared" si="13"/>
         <v>31.666666666666664</v>
       </c>
       <c r="J102" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>26.055555555555561</v>
       </c>
       <c r="K102" s="55">
         <v>18.600000000000001</v>
       </c>
       <c r="L102" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.21E-2</v>
       </c>
       <c r="M102" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.03E-2</v>
       </c>
       <c r="N102" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P102" s="10" t="s">
         <v>214</v>
       </c>
       <c r="Q102" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>5.3010000000000002</v>
       </c>
       <c r="R102" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38273</v>
       </c>
       <c r="S102" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>9</v>
       </c>
       <c r="T102" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.6520000000000001</v>
       </c>
       <c r="U102" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38076</v>
       </c>
       <c r="V102" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="W102" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>25.11</v>
       </c>
       <c r="X102" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37002</v>
       </c>
       <c r="Y102" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
       <c r="Z102" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.94</v>
       </c>
       <c r="AA102" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37975</v>
       </c>
       <c r="AB102" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>11</v>
       </c>
       <c r="AC102" s="53">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.1900000000000001E-2</v>
       </c>
       <c r="AD102" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37092</v>
       </c>
       <c r="AE102" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AF102" s="53"/>
@@ -6735,117 +6762,117 @@
         <v>60</v>
       </c>
       <c r="B103" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>7683</v>
       </c>
       <c r="C103" s="22">
+        <f t="shared" si="20"/>
+        <v>754</v>
+      </c>
+      <c r="D103" s="23">
+        <f t="shared" si="21"/>
+        <v>25392.718500000003</v>
+      </c>
+      <c r="E103" s="24">
+        <f t="shared" si="22"/>
+        <v>22196.756100000002</v>
+      </c>
+      <c r="F103" s="24">
+        <f t="shared" si="23"/>
+        <v>3195.9624000000003</v>
+      </c>
+      <c r="G103" s="53">
         <f t="shared" si="16"/>
-        <v>754</v>
-      </c>
-      <c r="D103" s="23">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="H103" s="54">
+        <f t="shared" si="16"/>
+        <v>3.0096857295247128</v>
+      </c>
+      <c r="I103" s="55">
         <f t="shared" si="17"/>
-        <v>25392.718500000003</v>
-      </c>
-      <c r="E103" s="24">
-        <f t="shared" si="18"/>
-        <v>22196.756100000002</v>
-      </c>
-      <c r="F103" s="24">
-        <f t="shared" si="19"/>
-        <v>3195.9624000000003</v>
-      </c>
-      <c r="G103" s="53">
-        <f t="shared" si="12"/>
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="H103" s="54">
-        <f t="shared" si="12"/>
-        <v>3.0096857295247128</v>
-      </c>
-      <c r="I103" s="55">
-        <f t="shared" si="13"/>
         <v>32.222222222222221</v>
       </c>
       <c r="J103" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>26.111111111111114</v>
       </c>
       <c r="K103" s="55">
         <v>18.46</v>
       </c>
       <c r="L103" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.1900000000000001E-2</v>
       </c>
       <c r="M103" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.01E-2</v>
       </c>
       <c r="N103" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P103" s="10" t="s">
         <v>206</v>
       </c>
       <c r="Q103" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>4.6520000000000001</v>
       </c>
       <c r="R103" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37696</v>
       </c>
       <c r="S103" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="T103" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.3940000000000001</v>
       </c>
       <c r="U103" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38082</v>
       </c>
       <c r="V103" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="W103" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15.94</v>
       </c>
       <c r="X103" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38178</v>
       </c>
       <c r="Y103" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="Z103" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.89</v>
       </c>
       <c r="AA103" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37975</v>
       </c>
       <c r="AB103" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="AC103" s="53">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.7999999999999996E-3</v>
       </c>
       <c r="AD103" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38075</v>
       </c>
       <c r="AE103" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="AF103" s="53"/>
@@ -6863,117 +6890,117 @@
         <v>162</v>
       </c>
       <c r="B104" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>8222</v>
       </c>
       <c r="C104" s="22">
+        <f t="shared" si="20"/>
+        <v>803</v>
+      </c>
+      <c r="D104" s="23">
+        <f t="shared" si="21"/>
+        <v>27721.104900000002</v>
+      </c>
+      <c r="E104" s="24">
+        <f t="shared" si="22"/>
+        <v>22533.234900000003</v>
+      </c>
+      <c r="F104" s="24">
+        <f t="shared" si="23"/>
+        <v>5187.8700000000008</v>
+      </c>
+      <c r="G104" s="53">
         <f t="shared" si="16"/>
-        <v>803</v>
-      </c>
-      <c r="D104" s="23">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="H104" s="54">
+        <f t="shared" si="16"/>
+        <v>3.0715905706371194</v>
+      </c>
+      <c r="I104" s="55">
         <f t="shared" si="17"/>
-        <v>27721.104900000002</v>
-      </c>
-      <c r="E104" s="24">
-        <f t="shared" si="18"/>
-        <v>22533.234900000003</v>
-      </c>
-      <c r="F104" s="24">
-        <f t="shared" si="19"/>
-        <v>5187.8700000000008</v>
-      </c>
-      <c r="G104" s="53">
-        <f t="shared" si="12"/>
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="H104" s="54">
-        <f t="shared" si="12"/>
-        <v>3.0715905706371194</v>
-      </c>
-      <c r="I104" s="55">
-        <f t="shared" si="13"/>
         <v>32.222222222222221</v>
       </c>
       <c r="J104" s="55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>26.166666666666664</v>
       </c>
       <c r="K104" s="55">
         <v>18.760000000000002</v>
       </c>
       <c r="L104" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.44E-2</v>
       </c>
       <c r="M104" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="N104" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101254.86534273588</v>
       </c>
       <c r="P104" s="10" t="s">
         <v>207</v>
       </c>
       <c r="Q104" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>5.6779999999999999</v>
       </c>
       <c r="R104" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38057</v>
       </c>
       <c r="S104" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="T104" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.5619999999999998</v>
       </c>
       <c r="U104" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38077</v>
       </c>
       <c r="V104" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="W104" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>20.11</v>
       </c>
       <c r="X104" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37732</v>
       </c>
       <c r="Y104" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="Z104" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.94</v>
       </c>
       <c r="AA104" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37975</v>
       </c>
       <c r="AB104" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>11</v>
       </c>
       <c r="AC104" s="53">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.38E-2</v>
       </c>
       <c r="AD104" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38083</v>
       </c>
       <c r="AE104" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="AF104" s="53"/>
@@ -6991,117 +7018,117 @@
         <v>163</v>
       </c>
       <c r="B105" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>5696</v>
       </c>
       <c r="C105" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>556</v>
       </c>
       <c r="D105" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>18244.595700000002</v>
       </c>
       <c r="E105" s="24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>13600.133100000001</v>
       </c>
       <c r="F105" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4644.4626000000007</v>
       </c>
       <c r="G105" s="53">
-        <f t="shared" ref="G105:H112" si="25">G189</f>
+        <f t="shared" ref="G105:H112" si="29">G189</f>
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="H105" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>2.9182014875239926</v>
       </c>
       <c r="I105" s="55">
-        <f t="shared" ref="I105:J110" si="26">(I189-32)/180*100</f>
+        <f t="shared" ref="I105:J110" si="30">(I189-32)/180*100</f>
         <v>31.666666666666664</v>
       </c>
       <c r="J105" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>26.055555555555561</v>
       </c>
       <c r="K105" s="55">
         <v>19.350000000000001</v>
       </c>
       <c r="L105" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.46E-2</v>
       </c>
       <c r="M105" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="N105" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101254.86534273588</v>
       </c>
       <c r="P105" s="10" t="s">
         <v>208</v>
       </c>
       <c r="Q105" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>6.0309999999999997</v>
       </c>
       <c r="R105" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38062</v>
       </c>
       <c r="S105" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="T105" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.8140000000000001</v>
       </c>
       <c r="U105" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38077</v>
       </c>
       <c r="V105" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="W105" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>35.06</v>
       </c>
       <c r="X105" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37732</v>
       </c>
       <c r="Y105" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="Z105" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.94</v>
       </c>
       <c r="AA105" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37975</v>
       </c>
       <c r="AB105" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="AC105" s="53">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="AD105" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37457</v>
       </c>
       <c r="AE105" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AF105" s="53"/>
@@ -7119,117 +7146,117 @@
         <v>164</v>
       </c>
       <c r="B106" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>5531</v>
       </c>
       <c r="C106" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>541</v>
       </c>
       <c r="D106" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17977.8747</v>
       </c>
       <c r="E106" s="24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>12831.624899999999</v>
       </c>
       <c r="F106" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>5146.2498000000005</v>
       </c>
       <c r="G106" s="53">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.12E-2</v>
       </c>
       <c r="H106" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>2.9607830533596839</v>
       </c>
       <c r="I106" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>31.111111111111111</v>
       </c>
       <c r="J106" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>25.944444444444446</v>
       </c>
       <c r="K106" s="55">
         <v>19.68</v>
       </c>
       <c r="L106" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.5699999999999999E-2</v>
       </c>
       <c r="M106" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.18E-2</v>
       </c>
       <c r="N106" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101254.86534273588</v>
       </c>
       <c r="P106" s="10" t="s">
         <v>209</v>
       </c>
       <c r="Q106" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.85</v>
       </c>
       <c r="R106" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38273</v>
       </c>
       <c r="S106" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>9</v>
       </c>
       <c r="T106" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.4980000000000002</v>
       </c>
       <c r="U106" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37466</v>
       </c>
       <c r="V106" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="W106" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>25.06</v>
       </c>
       <c r="X106" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37002</v>
       </c>
       <c r="Y106" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="Z106" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.94</v>
       </c>
       <c r="AA106" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37975</v>
       </c>
       <c r="AB106" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>11</v>
       </c>
       <c r="AC106" s="53">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>8.0999999999999996E-3</v>
       </c>
       <c r="AD106" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38188</v>
       </c>
       <c r="AE106" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AF106" s="53"/>
@@ -7247,117 +7274,117 @@
         <v>165</v>
       </c>
       <c r="B107" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4689</v>
       </c>
       <c r="C107" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>479</v>
       </c>
       <c r="D107" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>15914.450700000001</v>
       </c>
       <c r="E107" s="24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>11871.136200000001</v>
       </c>
       <c r="F107" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4043.3145000000004</v>
       </c>
       <c r="G107" s="53">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.11E-2</v>
       </c>
       <c r="H107" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.0794215750773994</v>
       </c>
       <c r="I107" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>28.333333333333332</v>
       </c>
       <c r="J107" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>25.5</v>
       </c>
       <c r="K107" s="55">
         <v>19.399999999999999</v>
       </c>
       <c r="L107" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.43E-2</v>
       </c>
       <c r="M107" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.1599999999999999E-2</v>
       </c>
       <c r="N107" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101254.86534273588</v>
       </c>
       <c r="P107" s="10" t="s">
         <v>210</v>
       </c>
       <c r="Q107" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.4550000000000001</v>
       </c>
       <c r="R107" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38107</v>
       </c>
       <c r="S107" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="T107" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.262</v>
       </c>
       <c r="U107" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>41120</v>
       </c>
       <c r="V107" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="W107" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15.11</v>
       </c>
       <c r="X107" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38138</v>
       </c>
       <c r="Y107" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="Z107" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.89</v>
       </c>
       <c r="AA107" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37975</v>
       </c>
       <c r="AB107" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="AC107" s="53">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>6.3E-3</v>
       </c>
       <c r="AD107" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38085</v>
       </c>
       <c r="AE107" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>8</v>
       </c>
       <c r="AF107" s="53"/>
@@ -7375,117 +7402,117 @@
         <v>166</v>
       </c>
       <c r="B108" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4855</v>
       </c>
       <c r="C108" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>503</v>
       </c>
       <c r="D108" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>17120.2641</v>
       </c>
       <c r="E108" s="24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>11534.071199999998</v>
       </c>
       <c r="F108" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>5586.1929000000009</v>
       </c>
       <c r="G108" s="53">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="H108" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.1952713885778277</v>
       </c>
       <c r="I108" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>27.222222222222221</v>
       </c>
       <c r="J108" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>25.333333333333329</v>
       </c>
       <c r="K108" s="55">
         <v>19.760000000000002</v>
       </c>
       <c r="L108" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.6400000000000001E-2</v>
       </c>
       <c r="M108" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.21E-2</v>
       </c>
       <c r="N108" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
       <c r="P108" s="11" t="s">
         <v>211</v>
       </c>
       <c r="Q108" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>4.4279999999999999</v>
       </c>
       <c r="R108" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38062</v>
       </c>
       <c r="S108" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="T108" s="25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2.722</v>
       </c>
       <c r="U108" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37467</v>
       </c>
       <c r="V108" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="W108" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>35</v>
       </c>
       <c r="X108" s="38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38098</v>
       </c>
       <c r="Y108" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="Z108" s="59">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.94</v>
       </c>
       <c r="AA108" s="30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>37975</v>
       </c>
       <c r="AB108" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="AC108" s="61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="AD108" s="38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>38188</v>
       </c>
       <c r="AE108" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AF108" s="61"/>
@@ -7503,54 +7530,54 @@
         <v>167</v>
       </c>
       <c r="B109" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3918</v>
       </c>
       <c r="C109" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>406</v>
       </c>
       <c r="D109" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>13445.083200000001</v>
       </c>
       <c r="E109" s="24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>9302.7008999999998</v>
       </c>
       <c r="F109" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4142.3823000000002</v>
       </c>
       <c r="G109" s="53">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="H109" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.1094086956521743</v>
       </c>
       <c r="I109" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>27.222222222222221</v>
       </c>
       <c r="J109" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>25.333333333333329</v>
       </c>
       <c r="K109" s="55">
         <v>19.760000000000002</v>
       </c>
       <c r="L109" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.6400000000000001E-2</v>
       </c>
       <c r="M109" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.21E-2</v>
       </c>
       <c r="N109" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
     </row>
@@ -7559,54 +7586,54 @@
         <v>168</v>
       </c>
       <c r="B110" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3823</v>
       </c>
       <c r="C110" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>399</v>
       </c>
       <c r="D110" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>13285.0506</v>
       </c>
       <c r="E110" s="24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>8973.8427000000011</v>
       </c>
       <c r="F110" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4311.2079000000003</v>
       </c>
       <c r="G110" s="53">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.14E-2</v>
       </c>
       <c r="H110" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.1466249644718145</v>
       </c>
       <c r="I110" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>26.666666666666668</v>
       </c>
       <c r="J110" s="55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>25.222222222222225</v>
       </c>
       <c r="K110" s="55">
         <v>19.8</v>
       </c>
       <c r="L110" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.67E-2</v>
       </c>
       <c r="M110" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="N110" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
     </row>
@@ -7615,31 +7642,31 @@
         <v>169</v>
       </c>
       <c r="B111" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3748</v>
       </c>
       <c r="C111" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>394</v>
       </c>
       <c r="D111" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>13192.137900000002</v>
       </c>
       <c r="E111" s="24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>8787.4311000000016</v>
       </c>
       <c r="F111" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4404.7068000000008</v>
       </c>
       <c r="G111" s="53">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.15E-2</v>
       </c>
       <c r="H111" s="54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.1849681071945923</v>
       </c>
       <c r="I111" s="55">
@@ -7654,15 +7681,15 @@
         <v>19.84</v>
       </c>
       <c r="L111" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.6899999999999998E-2</v>
       </c>
       <c r="M111" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.23E-2</v>
       </c>
       <c r="N111" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
     </row>
@@ -7671,31 +7698,31 @@
         <v>170</v>
       </c>
       <c r="B112" s="41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3880</v>
       </c>
       <c r="C112" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>407</v>
       </c>
       <c r="D112" s="42">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>13754.3037</v>
       </c>
       <c r="E112" s="43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>8799.7412999999997</v>
       </c>
       <c r="F112" s="43">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4954.5624000000007</v>
       </c>
       <c r="G112" s="61">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.17E-2</v>
       </c>
       <c r="H112" s="62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.2083750174947516</v>
       </c>
       <c r="I112" s="63">
@@ -7710,15 +7737,15 @@
         <v>20.059999999999999</v>
       </c>
       <c r="L112" s="60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.78E-2</v>
       </c>
       <c r="M112" s="57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.26E-2</v>
       </c>
       <c r="N112" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>101593.51037732697</v>
       </c>
     </row>
@@ -8688,7 +8715,7 @@
         <v>140223</v>
       </c>
       <c r="I147" s="25">
-        <f t="shared" ref="I147:I166" si="27">(F147)*0.2931/(C147)</f>
+        <f t="shared" ref="I147:I166" si="31">(F147)*0.2931/(C147)</f>
         <v>3.4174880051922543</v>
       </c>
       <c r="J147" s="95">
@@ -8778,7 +8805,7 @@
         <v>115136</v>
       </c>
       <c r="I148" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.4570510748065351</v>
       </c>
       <c r="J148" s="95">
@@ -8867,7 +8894,7 @@
         <v>128508</v>
       </c>
       <c r="I149" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.5364334687303032</v>
       </c>
       <c r="J149" s="95">
@@ -9045,7 +9072,7 @@
         <v>54446</v>
       </c>
       <c r="I151" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.235440710799268</v>
       </c>
       <c r="J151" s="95">
@@ -9134,7 +9161,7 @@
         <v>85002</v>
       </c>
       <c r="I152" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.705809741283383</v>
       </c>
       <c r="J152" s="95">
@@ -9223,7 +9250,7 @@
         <v>80478</v>
       </c>
       <c r="I153" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.2519060962192441</v>
       </c>
       <c r="J153" s="95">
@@ -9401,7 +9428,7 @@
         <v>69157</v>
       </c>
       <c r="I155" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.2175275351793013</v>
       </c>
       <c r="J155" s="95">
@@ -9490,7 +9517,7 @@
         <v>67435</v>
       </c>
       <c r="I156" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.2114691557976212</v>
       </c>
       <c r="J156" s="95">
@@ -9668,7 +9695,7 @@
         <v>62594</v>
       </c>
       <c r="I158" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.2265361707329006</v>
       </c>
       <c r="J158" s="95">
@@ -9842,7 +9869,7 @@
         <v>108196</v>
       </c>
       <c r="I160" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.5773999497976217</v>
       </c>
       <c r="J160" s="95">
@@ -10016,7 +10043,7 @@
         <v>62813</v>
       </c>
       <c r="I162" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.072773555555556</v>
       </c>
       <c r="J162" s="95">
@@ -10101,7 +10128,7 @@
         <v>62032</v>
       </c>
       <c r="I163" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.5279999190763922</v>
       </c>
       <c r="J163" s="95">
@@ -10182,7 +10209,7 @@
         <v>207</v>
       </c>
       <c r="I164" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>2.969354591186959</v>
       </c>
       <c r="J164" s="95">
@@ -10263,7 +10290,7 @@
         <v>365</v>
       </c>
       <c r="I165" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>2.6751863930517716</v>
       </c>
       <c r="J165" s="95">
@@ -10344,7 +10371,7 @@
         <v>87</v>
       </c>
       <c r="I166" s="25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3.2355450524842548</v>
       </c>
       <c r="J166" s="106">
@@ -10919,7 +10946,7 @@
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="H174" s="54">
-        <f t="shared" ref="H174:H196" si="28">D174*0.2931/B174</f>
+        <f t="shared" ref="H174:H196" si="32">D174*0.2931/B174</f>
         <v>3.4954391384051333</v>
       </c>
       <c r="I174" s="95">
@@ -11041,7 +11068,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="H175" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.541132144533083</v>
       </c>
       <c r="I175" s="95">
@@ -11163,7 +11190,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="H176" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.5410505644402641</v>
       </c>
       <c r="I176" s="95">
@@ -11283,7 +11310,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="H177" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.5374667365112624</v>
       </c>
       <c r="I177" s="95">
@@ -11403,7 +11430,7 @@
         <v>9.1999999999999998E-3</v>
       </c>
       <c r="H178" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.4218689799331106</v>
       </c>
       <c r="I178" s="95">
@@ -11523,7 +11550,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
       <c r="H179" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.1411533557046987</v>
       </c>
       <c r="I179" s="95">
@@ -11643,7 +11670,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="H180" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9516349137931037</v>
       </c>
       <c r="I180" s="95">
@@ -11763,7 +11790,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
       <c r="H181" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9729720608852395</v>
       </c>
       <c r="I181" s="95">
@@ -11883,7 +11910,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
       <c r="H182" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9987790181180602</v>
       </c>
       <c r="I182" s="95">
@@ -12003,7 +12030,7 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="H183" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9380927069425904</v>
       </c>
       <c r="I183" s="95">
@@ -12123,7 +12150,7 @@
         <v>1.0800000000000001E-2</v>
       </c>
       <c r="H184" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9362633593324872</v>
       </c>
       <c r="I184" s="95">
@@ -12243,7 +12270,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
       <c r="H185" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9567500452079569</v>
       </c>
       <c r="I185" s="95">
@@ -12325,11 +12352,11 @@
         <v>190</v>
       </c>
       <c r="AM185" s="30">
-        <f t="shared" ref="AM185:AN192" si="29">AM269</f>
+        <f t="shared" ref="AM185:AN192" si="33">AM269</f>
         <v>0</v>
       </c>
       <c r="AN185" s="115">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AO185" s="79" t="s">
@@ -12357,7 +12384,7 @@
         <v>0.01</v>
       </c>
       <c r="H186" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9472234003397513</v>
       </c>
       <c r="I186" s="95">
@@ -12439,11 +12466,11 @@
         <v>190</v>
       </c>
       <c r="AM186" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AN186" s="115">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AO186" s="79" t="s">
@@ -12471,7 +12498,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
       <c r="H187" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.0096857295247128</v>
       </c>
       <c r="I187" s="95">
@@ -12553,11 +12580,11 @@
         <v>190</v>
       </c>
       <c r="AM187" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AN187" s="115">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AO187" s="79" t="s">
@@ -12585,7 +12612,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
       <c r="H188" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.0715905706371194</v>
       </c>
       <c r="I188" s="95">
@@ -12667,11 +12694,11 @@
         <v>190</v>
       </c>
       <c r="AM188" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AN188" s="115">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AO188" s="79" t="s">
@@ -12699,7 +12726,7 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="H189" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9182014875239926</v>
       </c>
       <c r="I189" s="95">
@@ -12781,11 +12808,11 @@
         <v>190</v>
       </c>
       <c r="AM189" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AN189" s="115">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AO189" s="79" t="s">
@@ -12813,7 +12840,7 @@
         <v>1.12E-2</v>
       </c>
       <c r="H190" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2.9607830533596839</v>
       </c>
       <c r="I190" s="95">
@@ -12895,11 +12922,11 @@
         <v>190</v>
       </c>
       <c r="AM190" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AN190" s="115">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AO190" s="79" t="s">
@@ -12927,7 +12954,7 @@
         <v>1.11E-2</v>
       </c>
       <c r="H191" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.0794215750773994</v>
       </c>
       <c r="I191" s="95">
@@ -13009,11 +13036,11 @@
         <v>190</v>
       </c>
       <c r="AM191" s="30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AN191" s="115">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AO191" s="79" t="s">
@@ -13041,7 +13068,7 @@
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="H192" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.1952713885778277</v>
       </c>
       <c r="I192" s="95">
@@ -13123,11 +13150,11 @@
         <v>190</v>
       </c>
       <c r="AM192" s="38">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AN192" s="119">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AO192" s="80" t="s">
@@ -13155,7 +13182,7 @@
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="H193" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.1094086956521743</v>
       </c>
       <c r="I193" s="95">
@@ -13224,7 +13251,7 @@
         <v>1.14E-2</v>
       </c>
       <c r="H194" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.1466249644718145</v>
       </c>
       <c r="I194" s="95">
@@ -13291,7 +13318,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="H195" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.1849681071945923</v>
       </c>
       <c r="I195" s="95">
@@ -13358,7 +13385,7 @@
         <v>1.17E-2</v>
       </c>
       <c r="H196" s="54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.2083750174947516</v>
       </c>
       <c r="I196" s="129">

</xml_diff>